<commit_message>
pridani nekterych komponent pro regulaci
</commit_message>
<xml_diff>
--- a/nakupy/seznam FBR.xlsx
+++ b/nakupy/seznam FBR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents and Settings\BU2\Documents\bioreactor_KSnokhous\nakupy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB784528-22E8-4AA7-BE6A-8612539270B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21ACCF14-3D10-44E6-BD9E-827891E85C7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{BC32C59B-8597-4BC0-B079-46BEB167D570}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
   <si>
     <t>Název</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>driver pro krok. motor</t>
+  </si>
+  <si>
+    <t>display i2c</t>
+  </si>
+  <si>
+    <t>https://arduino-shop.cz/arduino/1421-eses-i2c-20x4-display-pro-jednodeskove-pocitace.html?gclid=Cj0KCQjwuL_8BRCXARIsAGiC51AaUN-iQm0k_3qSD826rhlR5hUuxtvJMt2UjPC1cdwT4N_Vt1o1S2saAtzAEALw_wcB</t>
   </si>
 </sst>
 </file>
@@ -659,8 +665,8 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,8 +1298,16 @@
         <v>238</v>
       </c>
       <c r="E33">
-        <f>(D33*1.19)</f>
-        <v>283.21999999999997</v>
+        <f>(D33*1.21)</f>
+        <v>287.98</v>
+      </c>
+      <c r="F33">
+        <f>(D33*C33)</f>
+        <v>714</v>
+      </c>
+      <c r="G33">
+        <f>(F33*1.21)</f>
+        <v>863.93999999999994</v>
       </c>
       <c r="H33" t="s">
         <v>73</v>
@@ -1310,8 +1324,16 @@
         <v>221.5</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E39" si="1">(D34*1.19)</f>
-        <v>263.58499999999998</v>
+        <f t="shared" ref="E34:E39" si="1">(D34*1.21)</f>
+        <v>268.01499999999999</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34:F39" si="2">(D34*C34)</f>
+        <v>664.5</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ref="G34:G39" si="3">(F34*1.21)</f>
+        <v>804.04499999999996</v>
       </c>
       <c r="H34" t="s">
         <v>75</v>
@@ -1329,7 +1351,15 @@
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
-        <v>40.912199999999999</v>
+        <v>41.599800000000002</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>171.9</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>207.999</v>
       </c>
       <c r="H35" t="s">
         <v>78</v>
@@ -1347,7 +1377,15 @@
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
-        <v>686.63</v>
+        <v>698.17</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>577</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>698.17</v>
       </c>
       <c r="H36" t="s">
         <v>79</v>
@@ -1365,21 +1403,57 @@
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
-        <v>322.60900000000004</v>
+        <v>328.03100000000001</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>271.10000000000002</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>328.03100000000001</v>
       </c>
       <c r="H37" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>276</v>
+      </c>
       <c r="E38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>333.96</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>552</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>667.92</v>
+      </c>
+      <c r="H38" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E39">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>